<commit_message>
update conv back prop (add inertia)
</commit_message>
<xml_diff>
--- a/step_by_step_mlp(inertia).xlsx
+++ b/step_by_step_mlp(inertia).xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="59">
   <si>
     <t xml:space="preserve">Input</t>
   </si>
@@ -51,121 +51,154 @@
     <t xml:space="preserve">Layer 1 (weights)</t>
   </si>
   <si>
+    <t xml:space="preserve">Transposed weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 1 (output)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derevative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 2 (weights)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 2 (output)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 3 (weights, final)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 3 (output, final)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back propagate (gradients)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Momentum (inertia)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 3 (Local Deltas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 3 (Sum(Delta*Weight) for layer 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 2 (Local Deltas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 2 (Sum(Delta*Weight) for layer 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 1 (Local Deltas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 1 (Sum(Delta*Weight) (do NOT NEED actually, because no layers before this one)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back propagate (update weights with inertia)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 1 (previous delta-weights)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 2 (previous delta-weights)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 3 (previous delta-weights)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 1 (delta-weights)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 1 (new weights)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 2 (delta-weights)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 2 (new weights)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 3 (delta-weights)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 3 (new weights)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Transposed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 1 (output)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derevative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 2 (weights)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 2 (output)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 3 (weights, final)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 3 (output, final)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desired</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Back propagate (gradients)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Learning Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Momentum (inertia)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 3 (Local Deltas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delta0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 3 (Sum(Delta*Weight) for layer 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 2 (Local Deltas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delta1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delta2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 2 (Sum(Delta*Weight) for layer 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 1 (Local Deltas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 1 (Sum(Delta*Weight) (do NOT NEED actually, because no layers before this one)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Back propagate (update weights with inertia)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 1 (previous delta-weights)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 2 (previous delta-weights)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 3 (previous delta-weights)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 1 (delta-weights)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 2 (delta-weights)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer 3 (delta-weights)</t>
   </si>
 </sst>
 </file>
@@ -308,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -333,8 +366,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -375,6 +408,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -469,7 +506,7 @@
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E68" activeCellId="0" sqref="E68"/>
+      <selection pane="topLeft" activeCell="H92" activeCellId="0" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -533,7 +570,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -631,7 +668,7 @@
         <v>0.305019996207409</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -775,7 +812,7 @@
         <v>0.563984529588071</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
@@ -1096,10 +1133,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>0</v>
@@ -1114,10 +1151,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>0</v>
@@ -1142,7 +1179,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B74" s="12"/>
       <c r="E74" s="13"/>
@@ -1152,10 +1189,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>0</v>
@@ -1170,10 +1207,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>0</v>
@@ -1188,10 +1225,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>0</v>
@@ -1216,7 +1253,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="12" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
@@ -1225,13 +1262,13 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>0</v>
@@ -1267,20 +1304,20 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="15" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B83" s="15"/>
       <c r="F83" s="16" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G83" s="16"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C84" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*B2*B62)+$B$40*C71</f>
@@ -1307,10 +1344,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C85" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*B2*B63)+$B$40*C72</f>
@@ -1337,20 +1374,20 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="15" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B87" s="15"/>
       <c r="F87" s="16" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G87" s="16"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C88" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$C$12*B53)+$B$40*C75</f>
@@ -1377,10 +1414,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C89" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$C$12*B54)+$B$40*C76</f>
@@ -1407,10 +1444,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C90" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$C$12*B55)+$B$40*C77</f>
@@ -1437,25 +1474,25 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="15" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
       <c r="H92" s="16" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I92" s="16"/>
       <c r="J92" s="16"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D93" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$B$45*C23)+$B$40*D80</f>
@@ -1532,12 +1569,12 @@
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
+      <selection pane="topLeft" activeCell="H92" activeCellId="0" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.89"/>
@@ -1599,8 +1636,8 @@
         <v>8</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="F6" s="6" t="s">
-        <v>9</v>
+      <c r="F6" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1701,8 +1738,8 @@
         <v>19</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="F16" s="6" t="s">
-        <v>9</v>
+      <c r="F16" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,8 +1889,8 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="H28" s="6" t="s">
-        <v>9</v>
+      <c r="H28" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2170,10 +2207,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C71" s="0" t="n">
         <f aca="false">Step_1!C84</f>
@@ -2190,10 +2227,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C72" s="0" t="n">
         <f aca="false">Step_1!C85</f>
@@ -2220,7 +2257,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B74" s="12"/>
       <c r="E74" s="13"/>
@@ -2230,10 +2267,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C75" s="0" t="n">
         <f aca="false">Step_1!C88</f>
@@ -2250,10 +2287,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C76" s="0" t="n">
         <f aca="false">Step_1!C89</f>
@@ -2270,10 +2307,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C77" s="0" t="n">
         <f aca="false">Step_1!C90</f>
@@ -2300,7 +2337,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="12" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
@@ -2309,13 +2346,13 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D80" s="0" t="n">
         <f aca="false">Step_1!D93</f>
@@ -2332,48 +2369,48 @@
       <c r="G80" s="13"/>
       <c r="H80" s="13"/>
     </row>
-    <row r="81" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="17"/>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-      <c r="H81" s="18"/>
-    </row>
-    <row r="82" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="17" t="n">
+    <row r="81" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="18"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="19"/>
+    </row>
+    <row r="82" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="18" t="n">
         <f aca="false">$B40</f>
         <v>0.6</v>
       </c>
-      <c r="B82" s="18" t="n">
+      <c r="B82" s="19" t="n">
         <f aca="false">B62</f>
         <v>-3.33452058942817</v>
       </c>
-      <c r="C82" s="18"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="18"/>
-      <c r="H82" s="18"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="19"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="15" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B83" s="15"/>
       <c r="F83" s="16" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G83" s="16"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C84" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*B2*B62)+$B$40*C71</f>
@@ -2400,10 +2437,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C85" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*B2*B63)+$B$40*C72</f>
@@ -2430,20 +2467,20 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="15" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B87" s="15"/>
       <c r="F87" s="16" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G87" s="16"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C88" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$C$12*B53)+$B$40*C75</f>
@@ -2470,10 +2507,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C89" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$C$12*B54)+$B$40*C76</f>
@@ -2500,10 +2537,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C90" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$C$12*B55)+$B$40*C77</f>
@@ -2530,25 +2567,25 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="15" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
       <c r="H92" s="16" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I92" s="16"/>
       <c r="J92" s="16"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D93" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$B$45*C23)+$B$40*D80</f>
@@ -2624,15 +2661,17 @@
   </sheetPr>
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O37" activeCellId="0" sqref="O37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J80" activeCellId="0" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2690,8 +2729,8 @@
         <v>8</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="F6" s="6" t="s">
-        <v>9</v>
+      <c r="F6" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2792,8 +2831,8 @@
         <v>19</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="F16" s="6" t="s">
-        <v>9</v>
+      <c r="F16" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,8 +2982,8 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="H28" s="6" t="s">
-        <v>9</v>
+      <c r="H28" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,10 +3300,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C71" s="0" t="n">
         <f aca="false">Step_2!C84</f>
@@ -3281,10 +3320,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C72" s="0" t="n">
         <f aca="false">Step_2!C85</f>
@@ -3311,7 +3350,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B74" s="12"/>
       <c r="E74" s="13"/>
@@ -3321,10 +3360,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C75" s="0" t="n">
         <f aca="false">Step_2!C88</f>
@@ -3341,10 +3380,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C76" s="0" t="n">
         <f aca="false">Step_2!C89</f>
@@ -3361,10 +3400,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C77" s="0" t="n">
         <f aca="false">Step_2!C90</f>
@@ -3391,7 +3430,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="12" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
@@ -3400,13 +3439,13 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D80" s="0" t="n">
         <f aca="false">Step_2!D93</f>
@@ -3445,20 +3484,20 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="15" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B83" s="15"/>
       <c r="F83" s="16" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G83" s="16"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C84" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*B2*B62)+$B$40*C71</f>
@@ -3485,10 +3524,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C85" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*B2*B63)+$B$40*C72</f>
@@ -3515,20 +3554,20 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="15" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B87" s="15"/>
       <c r="F87" s="16" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G87" s="16"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C88" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$C$12*B53)+$B$40*C75</f>
@@ -3555,10 +3594,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C89" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$C$12*B54)+$B$40*C76</f>
@@ -3585,10 +3624,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C90" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$C$12*B55)+$B$40*C77</f>
@@ -3615,25 +3654,25 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="15" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
       <c r="H92" s="16" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I92" s="16"/>
       <c r="J92" s="16"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D93" s="0" t="n">
         <f aca="false">(1-$B$40)*-($B$39*$B$45*C23)+$B$40*D80</f>

</xml_diff>

<commit_message>
add and sub functions for tensor need to be refactored
</commit_message>
<xml_diff>
--- a/step_by_step_mlp(inertia).xlsx
+++ b/step_by_step_mlp(inertia).xlsx
@@ -505,7 +505,7 @@
   </sheetPr>
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H92" activeCellId="0" sqref="H92"/>
     </sheetView>
   </sheetViews>
@@ -2661,15 +2661,16 @@
   </sheetPr>
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J80" activeCellId="0" sqref="J80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>

</xml_diff>